<commit_message>
update supp data revision 2
</commit_message>
<xml_diff>
--- a/Supplemental_Data/Supplemental_Dataset_7.xlsx
+++ b/Supplemental_Data/Supplemental_Dataset_7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27706"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/engje/Documents/Data/U54-TMA-9/Liver_Lung_PDAC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69900772-BE17-D341-84C7-A7F4C77C76AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{69900772-BE17-D341-84C7-A7F4C77C76AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73FFF5E3-51A6-49D0-B893-239866E63505}"/>
   <bookViews>
-    <workbookView xWindow="11120" yWindow="500" windowWidth="27580" windowHeight="17500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11120" yWindow="500" windowWidth="27580" windowHeight="17500" firstSheet="4" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample_avg_density" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,28 @@
     <sheet name="cell_type_gating" sheetId="4" r:id="rId4"/>
     <sheet name="lymphoid_aggregates" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="87">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -155,6 +171,9 @@
     <t>Lung</t>
   </si>
   <si>
+    <t>low</t>
+  </si>
+  <si>
     <t>ST-00019367</t>
   </si>
   <si>
@@ -167,9 +186,6 @@
     <t>ST-00020181</t>
   </si>
   <si>
-    <t>low</t>
-  </si>
-  <si>
     <t>ST-00017078</t>
   </si>
   <si>
@@ -200,6 +216,12 @@
     <t>p.value</t>
   </si>
   <si>
+    <t>FDR significance</t>
+  </si>
+  <si>
+    <t>FDR</t>
+  </si>
+  <si>
     <t>CD8.T.cells</t>
   </si>
   <si>
@@ -221,27 +243,24 @@
     <t>B.cells</t>
   </si>
   <si>
+    <t>Mature.DC</t>
+  </si>
+  <si>
+    <t>Immature.DC</t>
+  </si>
+  <si>
+    <t>low_pORG</t>
+  </si>
+  <si>
+    <t>high_pORG</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
     <t>*</t>
   </si>
   <si>
-    <t>Mature.DC</t>
-  </si>
-  <si>
-    <t>Immature.DC</t>
-  </si>
-  <si>
-    <t>low_pORG</t>
-  </si>
-  <si>
-    <t>high_pORG</t>
-  </si>
-  <si>
-    <t>**</t>
-  </si>
-  <si>
-    <t>Number of Imm.agg</t>
-  </si>
-  <si>
     <r>
       <t>CD45</t>
     </r>
@@ -1602,6 +1621,9 @@
       </rPr>
       <t xml:space="preserve">- </t>
     </r>
+  </si>
+  <si>
+    <t>Number of lymphoid.agg</t>
   </si>
 </sst>
 </file>
@@ -2508,11 +2530,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
     <row r="1" spans="1:38">
       <c r="A1" t="s">
@@ -2630,7 +2652,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="17">
+    <row r="2" spans="1:38" ht="17.100000000000001">
       <c r="A2">
         <v>1127</v>
       </c>
@@ -2746,7 +2768,7 @@
         <v>46.972479579999998</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="17">
+    <row r="3" spans="1:38" ht="17.100000000000001">
       <c r="A3">
         <v>1749</v>
       </c>
@@ -2769,7 +2791,7 @@
         <v>42</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I3">
         <v>3246.2703080000001</v>
@@ -2862,12 +2884,12 @@
         <v>36.692071800000001</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="17">
+    <row r="4" spans="1:38" ht="17.100000000000001">
       <c r="A4">
         <v>6951</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C4">
         <v>-0.45060012100000002</v>
@@ -2885,7 +2907,7 @@
         <v>39</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I4">
         <v>4055.0989249999998</v>
@@ -2978,12 +3000,12 @@
         <v>15.094711</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="17">
+    <row r="5" spans="1:38" ht="17.100000000000001">
       <c r="A5">
         <v>7080</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C5">
         <v>0.34118491200000001</v>
@@ -3094,12 +3116,12 @@
         <v>1.4662466460000001</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="17">
+    <row r="6" spans="1:38" ht="17.100000000000001">
       <c r="A6">
         <v>8049</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C6">
         <v>0.301062414</v>
@@ -3210,12 +3232,12 @@
         <v>84.898445140000007</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="17">
+    <row r="7" spans="1:38" ht="17.100000000000001">
       <c r="A7">
         <v>8122</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C7">
         <v>0.45187851899999998</v>
@@ -3326,7 +3348,7 @@
         <v>14.8967559</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="17">
+    <row r="8" spans="1:38" ht="17.100000000000001">
       <c r="A8">
         <v>15475</v>
       </c>
@@ -3349,7 +3371,7 @@
         <v>39</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I8">
         <v>4883.0256550000004</v>
@@ -3442,7 +3464,7 @@
         <v>26.73836545</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="17">
+    <row r="9" spans="1:38" ht="17.100000000000001">
       <c r="A9">
         <v>18268</v>
       </c>
@@ -3558,7 +3580,7 @@
         <v>5.2024463909999996</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="17">
+    <row r="10" spans="1:38" ht="17.100000000000001">
       <c r="A10">
         <v>19234</v>
       </c>
@@ -3674,7 +3696,7 @@
         <v>17.402114640000001</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="17">
+    <row r="11" spans="1:38" ht="17.100000000000001">
       <c r="A11">
         <v>164354</v>
       </c>
@@ -3697,7 +3719,7 @@
         <v>42</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I11">
         <v>18899.98171</v>
@@ -3790,7 +3812,7 @@
         <v>25.612572459999999</v>
       </c>
     </row>
-    <row r="12" spans="1:38" ht="17">
+    <row r="12" spans="1:38" ht="17.100000000000001">
       <c r="A12">
         <v>232215</v>
       </c>
@@ -3906,7 +3928,7 @@
         <v>21.751736080000001</v>
       </c>
     </row>
-    <row r="13" spans="1:38" ht="17">
+    <row r="13" spans="1:38" ht="17.100000000000001">
       <c r="A13">
         <v>248041</v>
       </c>
@@ -3929,7 +3951,7 @@
         <v>42</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I13">
         <v>3672.8013059999998</v>
@@ -4029,15 +4051,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -4050,146 +4072,176 @@
       <c r="D1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D2">
         <v>0.156317606301423</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75">
       <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D3" s="3">
         <v>8.4859412097966095E-14</v>
       </c>
       <c r="E3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="3">
+        <v>7.6399999999999998E-13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
       </c>
       <c r="D4" s="3">
         <v>2.37451080620304E-9</v>
       </c>
       <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1.07E-8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
       </c>
       <c r="D5">
         <v>4.6186823269047902E-4</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>64</v>
+      </c>
+      <c r="F5">
+        <v>1.0399999999999999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D6">
         <v>0.40254582146281997</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6">
+        <v>0.45300000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D7">
         <v>3.90252830828757E-2</v>
       </c>
-      <c r="E7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7">
+        <v>7.0199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D8">
         <v>0.374874376750504</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <v>0.45300000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D9">
         <v>0.98372525776236397</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9">
+        <v>0.98399999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D10">
         <v>1.1353174364408301E-4</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="F10">
+        <v>3.4099999999999999E-4</v>
       </c>
     </row>
   </sheetData>
@@ -4199,15 +4251,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <cols>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -4220,152 +4275,185 @@
       <c r="D1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D2">
         <v>0.32718847978981902</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>0.32700000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D3" s="3">
         <v>4.3701734648554097E-6</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>64</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1.9700000000000001E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D4">
         <v>2.0176714377438299E-4</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>64</v>
+      </c>
+      <c r="F4">
+        <v>6.0499999999999996E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D5">
         <v>2.6714417385045302E-3</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>71</v>
+      </c>
+      <c r="F5">
+        <v>6.0099999999999997E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D6">
         <v>5.4023570445633296E-3</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>71</v>
+      </c>
+      <c r="F6">
+        <v>9.7199999999999995E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D7">
         <v>0.27716940778888699</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7">
+        <v>0.312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D8">
         <v>3.84894615710916E-2</v>
       </c>
       <c r="E8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>72</v>
+      </c>
+      <c r="F8">
+        <v>4.9500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D9">
         <v>2.2766419127289401E-2</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>72</v>
+      </c>
+      <c r="F9">
+        <v>3.4099999999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D10" s="3">
         <v>6.0461952609634798E-7</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="F10" s="3">
+        <v>5.4500000000000003E-6</v>
       </c>
     </row>
   </sheetData>
@@ -4381,113 +4469,113 @@
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17">
+    <row r="1" spans="1:2" ht="17.100000000000001">
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.100000000000001">
       <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.100000000000001">
       <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.100000000000001">
       <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="17">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.100000000000001">
       <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="17">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.100000000000001">
       <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="17">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.100000000000001">
       <c r="A7" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="17">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="17.100000000000001">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="17">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="17.100000000000001">
       <c r="A9" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="17">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="17.100000000000001">
       <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="17">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="17.100000000000001">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="17">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="17.100000000000001">
       <c r="A12" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="17">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="17.100000000000001">
       <c r="A13" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -4499,18 +4587,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="33.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.375" customWidth="1"/>
+    <col min="2" max="2" width="21.125" customWidth="1"/>
+    <col min="3" max="3" width="33.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20">
+    <row r="1" spans="1:3" ht="18.75">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4518,147 +4606,147 @@
         <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="20">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="20.100000000000001">
       <c r="A2" s="5">
         <v>1127</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C2" s="5">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20">
+    <row r="3" spans="1:3" ht="20.100000000000001">
       <c r="A3" s="5">
         <v>8049</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C3" s="5">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20">
+    <row r="4" spans="1:3" ht="20.100000000000001">
       <c r="A4" s="5">
         <v>8122</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C4" s="5">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20">
+    <row r="5" spans="1:3" ht="20.100000000000001">
       <c r="A5" s="5">
         <v>18268</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C5" s="5">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20">
+    <row r="6" spans="1:3" ht="20.100000000000001">
       <c r="A6" s="5">
         <v>19234</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C6" s="5">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="20">
+    <row r="7" spans="1:3" ht="20.100000000000001">
       <c r="A7" s="5">
         <v>6951</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C7" s="5">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20">
+    <row r="8" spans="1:3" ht="20.100000000000001">
       <c r="A8" s="5">
         <v>7080</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20">
+    <row r="9" spans="1:3" ht="20.100000000000001">
       <c r="A9" s="5">
         <v>9286</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C9" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="20">
+    <row r="10" spans="1:3" ht="20.100000000000001">
       <c r="A10" s="5">
         <v>15475</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C10" s="5">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="20">
+    <row r="11" spans="1:3" ht="20.100000000000001">
       <c r="A11" s="5">
         <v>232215</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C11" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20">
+    <row r="12" spans="1:3" ht="20.100000000000001">
       <c r="A12" s="5">
         <v>248041</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20">
+    <row r="13" spans="1:3" ht="20.100000000000001">
       <c r="A13" s="5">
         <v>1749</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C13" s="5">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="20">
+    <row r="14" spans="1:3" ht="20.100000000000001">
       <c r="A14" s="5">
         <v>164354</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C14" s="5">
         <v>46</v>

</xml_diff>